<commit_message>
doc(command) : Add a documentation to the commands.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_cmd.xlsx
+++ b/fichiers_xls/test_cmd.xlsx
@@ -91,7 +91,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -162,6 +162,11 @@
         <fgColor rgb="00163e6a"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000a933"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -182,7 +187,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -308,6 +313,9 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -485,7 +493,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -648,7 +656,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -700,7 +708,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -829,7 +837,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -992,7 +1000,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1044,7 +1052,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1174,7 +1182,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -1337,7 +1345,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1389,7 +1397,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1519,7 +1527,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -1682,7 +1690,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1734,7 +1742,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -2183,7 +2191,7 @@
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="16.2" customWidth="1" style="21" min="6" max="6"/>
     <col width="14.38" customWidth="1" style="22" min="7" max="7"/>
@@ -7334,7 +7342,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="21" min="1" max="1024"/>
   </cols>
@@ -7686,7 +7694,7 @@
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="21" min="1" max="1024"/>
   </cols>
@@ -8011,7 +8019,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.08" customWidth="1" style="21" min="1" max="1"/>
     <col width="11.52" customWidth="1" style="21" min="942" max="1024"/>
@@ -8192,7 +8200,7 @@
       <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="21" min="1" max="1024"/>
   </cols>
@@ -8594,7 +8602,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="21" min="1" max="1024"/>
   </cols>
@@ -8996,7 +9004,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.52" customWidth="1" style="21" min="1021" max="1024"/>
   </cols>
@@ -10098,7 +10106,7 @@
       <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.84" customWidth="1" style="21" min="1" max="1024"/>
   </cols>
@@ -10178,37 +10186,37 @@
       </c>
     </row>
     <row r="3" ht="16.05" customHeight="1" s="24">
-      <c r="A3" s="21" t="inlineStr">
+      <c r="A3" s="43" t="inlineStr">
         <is>
           <t>Abdel Moneim</t>
         </is>
       </c>
-      <c r="B3" s="41" t="inlineStr">
+      <c r="B3" s="43" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C3" s="21" t="inlineStr">
+      <c r="C3" s="43" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D3" s="21" t="inlineStr">
+      <c r="D3" s="43" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E3" s="41" t="inlineStr">
+      <c r="E3" s="43" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="F3" s="21" t="inlineStr">
+      <c r="F3" s="43" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G3" s="21" t="inlineStr">
+      <c r="G3" s="43" t="inlineStr">
         <is>
           <t>7 min 22 s</t>
         </is>
@@ -10289,37 +10297,37 @@
       </c>
     </row>
     <row r="6" ht="16.05" customHeight="1" s="24">
-      <c r="A6" s="21" t="inlineStr">
+      <c r="A6" s="43" t="inlineStr">
         <is>
           <t>Abdelali</t>
         </is>
       </c>
-      <c r="B6" s="41" t="inlineStr">
+      <c r="B6" s="43" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="C6" s="21" t="inlineStr">
+      <c r="C6" s="43" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D6" s="21" t="inlineStr">
+      <c r="D6" s="43" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E6" s="41" t="inlineStr">
+      <c r="E6" s="43" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="F6" s="21" t="inlineStr">
+      <c r="F6" s="43" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="G6" s="21" t="inlineStr">
+      <c r="G6" s="43" t="inlineStr">
         <is>
           <t>7 min 44 s</t>
         </is>
@@ -10363,37 +10371,37 @@
       </c>
     </row>
     <row r="8" ht="16.05" customHeight="1" s="24">
-      <c r="A8" s="21" t="inlineStr">
+      <c r="A8" s="43" t="inlineStr">
         <is>
           <t>Abdelkarim</t>
         </is>
       </c>
-      <c r="B8" s="42" t="inlineStr">
+      <c r="B8" s="43" t="inlineStr">
         <is>
           <t>Yacine</t>
         </is>
       </c>
-      <c r="C8" s="21" t="inlineStr">
+      <c r="C8" s="43" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D8" s="21" t="inlineStr">
+      <c r="D8" s="43" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E8" s="42" t="inlineStr">
+      <c r="E8" s="43" t="inlineStr">
         <is>
           <t>Yacine</t>
         </is>
       </c>
-      <c r="F8" s="21" t="inlineStr">
+      <c r="F8" s="43" t="inlineStr">
         <is>
           <t>8,07</t>
         </is>
       </c>
-      <c r="G8" s="21" t="inlineStr">
+      <c r="G8" s="43" t="inlineStr">
         <is>
           <t>4 min 17 s</t>
         </is>
@@ -10649,7 +10657,7 @@
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="21" min="1" max="2"/>
     <col width="11.52" customWidth="1" style="21" min="995" max="1024"/>
@@ -10767,7 +10775,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="21" min="1" max="3"/>
     <col width="21.53" customWidth="1" style="21" min="4" max="4"/>

</xml_diff>